<commit_message>
task #21 Some more test for RowAutofitUtil
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/rows_autofit_util.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/rows_autofit_util.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Row with standard font</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>Row with very huge font</t>
+  </si>
+  <si>
+    <t>Row with very small font and very small height</t>
   </si>
 </sst>
 </file>
@@ -82,10 +85,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -366,13 +372,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A4"/>
+  <dimension ref="A2:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="238" zoomScaleNormal="238" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -384,9 +393,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="61.5" x14ac:dyDescent="0.9">
+    <row r="4" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A4" s="2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.9">
+      <c r="A8" s="3">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
task #21 Tests for reading/writing customHeight attribute. Setup method changed to @BeforeClass to @Before since multiple tests modifying the same spreadsheet row
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/rows_autofit_util.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/rows_autofit_util.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Row with standard font</t>
   </si>
@@ -36,6 +36,15 @@
   </si>
   <si>
     <t>Row with very small font and very small height</t>
+  </si>
+  <si>
+    <t>Multiline text that goes on two rows</t>
+  </si>
+  <si>
+    <t>Multiline text that goes on three rows bla</t>
+  </si>
+  <si>
+    <t>Single line text</t>
   </si>
 </sst>
 </file>
@@ -85,13 +94,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,40 +385,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A8"/>
+  <dimension ref="A2:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="238" zoomScaleNormal="238" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="238" zoomScaleNormal="238" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="29.25" customHeight="1" x14ac:dyDescent="0.9">
+    <row r="4" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.9">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.9">
       <c r="A8" s="3">
         <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>123</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="5">
+        <v>43041</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
task #21 Committed reference file for RowsAutofitUtilTest
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/rows_autofit_util.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/rows_autofit_util.xlsx
@@ -387,8 +387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="238" zoomScaleNormal="238" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="238" zoomScaleNormal="238" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +424,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -434,7 +434,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>

</xml_diff>